<commit_message>
Adding a new article to document
</commit_message>
<xml_diff>
--- a/Article Searches/Reading.xlsx
+++ b/Article Searches/Reading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="315" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B34A5DF-1534-463E-B8A4-95C167447AFC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -715,7 +715,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1255,20 +1255,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="105" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="105" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="45.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="149.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="149.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="92.25" customHeight="1">
+    <row r="2" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>6</v>
@@ -1306,7 +1306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="60.75" customHeight="1">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="7" t="s">
         <v>10</v>
@@ -1324,7 +1324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="93" customHeight="1">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="7" t="s">
         <v>14</v>
@@ -1342,7 +1342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="195" customHeight="1">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
         <v>18</v>
@@ -1360,7 +1360,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="147.75" customHeight="1">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
         <v>22</v>
@@ -1378,7 +1378,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="135" customHeight="1">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="7" t="s">
         <v>25</v>
@@ -1396,7 +1396,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="220.5" customHeight="1">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="220.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
         <v>29</v>
@@ -1414,7 +1414,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="79.5" customHeight="1">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="7" t="s">
         <v>33</v>
@@ -1432,7 +1432,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="105" customHeight="1">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20"/>
       <c r="B10" s="11" t="s">
         <v>37</v>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="105" customHeight="1">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
         <v>40</v>
@@ -1466,7 +1466,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="16" customFormat="1" ht="105" customHeight="1">
+    <row r="12" spans="1:6" s="16" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Updated to include work in challenges
</commit_message>
<xml_diff>
--- a/Article Searches/Reading.xlsx
+++ b/Article Searches/Reading.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="315" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B34A5DF-1534-463E-B8A4-95C167447AFC}"/>
+  <xr:revisionPtr revIDLastSave="444" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{886A7D61-27FD-44E3-8867-E365722EF156}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Articles" sheetId="1" r:id="rId1"/>
+    <sheet name="Challenges" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="refence11">Articles!$A$12:$A$12</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+  <si>
+    <t>Ref</t>
+  </si>
   <si>
     <t>GBU</t>
   </si>
@@ -664,7 +671,7 @@
 • The bottleneck is more sever is a distrinuted MTL network</t>
   </si>
   <si>
-    <t>Communication and computation efficiency in Federated Learning: A Surbvey</t>
+    <t>Communication and computation efficiency in Federated Learning: A Survey</t>
   </si>
   <si>
     <t>Omair Rashed Abdulwareth Almanifi</t>
@@ -709,13 +716,217 @@
       <t>This overhead is made worse as the number of clients increases, slowing down the process even further
 • Most FL applications, especially those involving IoT, the clients are devices with limited computatuinal capacity, such as microcontrollers, and microprocessors, used in Unmanned Aerial Vehicles (AUVs), smart home appliences, and smart wearables. While most serverssare equipped with state of the art TPUs or GPU, the clients will often have inferior processing units, that are often occupied with other tasts besides model training</t>
     </r>
+  </si>
+  <si>
+    <t>Comms</t>
+  </si>
+  <si>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Deeper</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Expensive communications</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>System heterogeneity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Devices can have various 
+• CPUs, GPUs, and RAM,
+• As well as various network connectivity schemes (3G, 4G, 5G, WiFi)
+• Fluctuarions in power capacity
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">• These elements give rise to statistical heterogeneity
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Could make scalling up a problem</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Constant comminication between server and devices for updates can result in:
+• Bottlenecks due to limited bandwidth
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This can increase costs</t>
+    </r>
+  </si>
+  <si>
+    <t>Asynchronous comms</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Typical scheme is synchronous comms
+• This can be hindered by constraints on participant devices' computational resources, and tx bandwidth
+• This can lead to disruptions in learning
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">An alternative approach is asumchronous comms -- asynch training and asymch tx to the server
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>• This approach can help reduce bottlenecks</t>
+    </r>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Client selection</t>
+  </si>
+  <si>
+    <t>• The desire is to select the clients who will 
+• Neither delay nor disrupt the aggregation phase due to issues with resources
+• This also reduces the chances of the devices traiggering system failures due to their own malfunctions
+• Methods so car have issues (e.g., random selection could still include devices with limited resources or poor data)</t>
+  </si>
+  <si>
+    <t>A systematic Review of Federted Leaning: Challenges, Aggregation Methodss, and Development Tools</t>
+  </si>
+  <si>
+    <t>Badra Souhial Guendouzi</t>
+  </si>
+  <si>
+    <t>Journal of Network and Computer Applications</t>
+  </si>
+  <si>
+    <t>Fault tolerance</t>
+  </si>
+  <si>
+    <t>Aims to keep an uniterrupted leanring process
+• Desite HW or SW failures or malfunctions
+• Ideas like checkpointing, heartbeat monitoring, redundant processing, error detection and correction have been implemented to various degrees of success</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Data/Statistical heterogeneity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is the situation where the data distribution is different across different devices (clients or server)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> In the form of non-identical and independently distrinuted (non-IID) data, belonging to the devices
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>• Domain shift: where local datasets possess various characteristcs and features - these disparities can impact performance and convergence
+• An example would be two system to monitor accents, running the same model, with one device located in Cork, and another in Paris</t>
+    </r>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Model heterogeneity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since the number if IoT sensors can be very large, and can differ across verious scenarios
+• Leading to a range of datasets, and their associated models
+• Different device resources could meab a device cannot run a more intersive model (see System, above)
+</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>The objective is to ensure that the data is private along and transactions are secure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -809,6 +1020,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -833,7 +1056,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -843,17 +1066,41 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -863,30 +1110,44 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -896,25 +1157,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1253,238 +1530,722 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="105" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="45.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="149.44140625" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="149.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10">
         <v>2024</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2023</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="24">
+        <v>2023</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2021</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2024</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="10">
+        <v>2023</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="220.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2023</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="10">
+        <v>2023</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="7" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2023</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="10">
+        <v>2023</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="D3" s="19">
+      <c r="B12" s="16"/>
+      <c r="C12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="10">
         <v>2023</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="19">
+      <c r="B13" s="20"/>
+      <c r="C13" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="7">
         <v>2023</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="195" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="19">
-        <v>2021</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="19">
-        <v>2024</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="19">
-        <v>2023</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="220.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="19">
-        <v>2023</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="19">
-        <v>2023</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="12">
-        <v>2023</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="19">
-        <v>2023</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="16" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="18">
-        <v>2023</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>47</v>
-      </c>
+      <c r="F13" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="20"/>
+    </row>
+    <row r="37" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="20"/>
+    </row>
+    <row r="38" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="20"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="20"/>
+    </row>
+    <row r="39" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="20"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="20"/>
+    </row>
+    <row r="41" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="45" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8B0AD9-241F-48FB-91B9-FA2C6942572D}">
+  <dimension ref="C2:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="120.21875" customWidth="1"/>
+    <col min="6" max="6" width="8" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C3" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="C4" s="28"/>
+      <c r="D4" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C7" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
formatting changes more than anything
</commit_message>
<xml_diff>
--- a/Article Searches/Reading.xlsx
+++ b/Article Searches/Reading.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="468" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4149D6A0-92B6-427A-9C48-CB6F681AB527}"/>
+  <xr:revisionPtr revIDLastSave="629" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB06C783-84A7-4893-A3D2-9E71523E2C3D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles" sheetId="1" r:id="rId1"/>
     <sheet name="Challenges" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="refence11">Articles!$A$12:$A$12</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>Ref</t>
   </si>
@@ -232,7 +233,7 @@
     </r>
   </si>
   <si>
-    <t>Blockchain-Based Federated Leaning for Device Failure Detection in Industrial IoT</t>
+    <t>Blockchain-Based Federated Learning for Device Failure Detection in Industrial IoT</t>
   </si>
   <si>
     <t>Weisham Zhang</t>
@@ -718,19 +719,92 @@
     </r>
   </si>
   <si>
+    <t>A systematic Review of Federted Leaning: Challenges, Aggregation Methodss, and Development Tools</t>
+  </si>
+  <si>
+    <t>Badra Souhial Guendouzi</t>
+  </si>
+  <si>
+    <t>Journal of Network and Computer Applications</t>
+  </si>
+  <si>
+    <t>Model Optimisation Techniques im Personal Federated Learning: A Survey</t>
+  </si>
+  <si>
+    <t>Fahad Sabah</t>
+  </si>
+  <si>
+    <t>Expert System with Application</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>Comms</t>
   </si>
   <si>
-    <t>Heading</t>
-  </si>
-  <si>
-    <t>Deeper</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>Expensive communications</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Constant comminication between server and devices for updates can result in:
+• Bottlenecks due to limited bandwidth
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This can increase costs</t>
+    </r>
+  </si>
+  <si>
+    <t>Asynchronous comms</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Typical scheme is synchronous comms
+• This can be hindered by constraints on participant devices' computational resources, and tx bandwidth
+• This can lead to disruptions in learning
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">An alternative approach is asumchronous comms -- asynch training and asymch tx to the server
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>• This approach can help reduce bottlenecks</t>
+    </r>
+  </si>
+  <si>
+    <t>Limited commumications</t>
+  </si>
+  <si>
+    <t>6/7</t>
   </si>
   <si>
     <t>System</t>
@@ -782,55 +856,38 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Constant comminication between server and devices for updates can result in:
-• Bottlenecks due to limited bandwidth
+    <t>Fault tolerance</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Aims to keep an uniterrupted leanring process
+• Despite HW or SW failures or malfunctions
+• Ideas like checkpointing, heartbeat monitoring, redundant processing, error detection and correction have been implemented to various degrees of success
 • </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This can increase costs</t>
-    </r>
-  </si>
-  <si>
-    <t>Asynchronous comms</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Typical scheme is synchronous comms
-• This can be hindered by constraints on participant devices' computational resources, and tx bandwidth
-• This can lead to disruptions in learning
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">An alternative approach is asumchronous comms -- asynch training and asymch tx to the server
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>• This approach can help reduce bottlenecks</t>
-    </r>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Systems should remain resilient to single or coordianted failures for a "reasonable" fraction of clients -- more important when the device numbers are smaller</t>
+    </r>
+  </si>
+  <si>
+    <t>Scalability</t>
+  </si>
+  <si>
+    <t>Massively distributed nature</t>
+  </si>
+  <si>
+    <t>This is a problem that is probably connected with the lack of research done on the scalability issue</t>
   </si>
   <si>
     <t>Client</t>
@@ -845,27 +902,134 @@
 • Methods so car have issues (e.g., random selection could still include devices with limited resources or poor data)</t>
   </si>
   <si>
-    <t>A systematic Review of Federted Leaning: Challenges, Aggregation Methodss, and Development Tools</t>
-  </si>
-  <si>
-    <t>Badra Souhial Guendouzi</t>
-  </si>
-  <si>
-    <t>Journal of Network and Computer Applications</t>
-  </si>
-  <si>
-    <t>Fault tolerance</t>
-  </si>
-  <si>
-    <t>Aims to keep an uniterrupted leanring process
-• Desite HW or SW failures or malfunctions
-• Ideas like checkpointing, heartbeat monitoring, redundant processing, error detection and correction have been implemented to various degrees of success</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
+    <t>Multimodal data sources</t>
+  </si>
+  <si>
+    <t>Multimodal dats is data the comes from a number of sources, such as audio, video, temperature etc.</t>
+  </si>
+  <si>
     <t>Data/Statistical heterogeneity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is the situation where the data distribution is different across different devices (clients or server)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> In the form of non-identical and independently distrinuted (non-IID) data, belonging to the devices
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">• Domain shift: where local datasets possess various characteristcs and features - these disparities can impact performance and convergence
+• An example would be two system to monitor accents, running the same model, with one device located in Cork, and another in Paris
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Imbalanced data distribution can lead to statistical heterogeneity</t>
+    </r>
+  </si>
+  <si>
+    <t>Non-IID</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Non-Independent and Identically Distributed Data (Non-IID) data is a significant challenge if FL:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Models being updated with Independent and Identically Distributed (IID) data is a typical assumtion of FL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>• But this is not what happens in real life
+• Assuming IID, and getting Non-IID can greatly increase the training complexity</t>
+    </r>
+  </si>
+  <si>
+    <t>Imblanced Data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Some clients can produce more data than others, and sometimes this difference can be significant, and this can be a challenge:
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Imbalanced data distribution can lead to statistical heterogeneity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• Will lead to an increase in training complexity</t>
+    </r>
   </si>
   <si>
     <t>Model</t>
@@ -878,6 +1042,18 @@
 • Leading to a range of datasets, and their associated models
 • Different device resources could meab a device cannot run a more intersive model (see System, above)
 </t>
+  </si>
+  <si>
+    <t>Neighbour dependency</t>
+  </si>
+  <si>
+    <t>With topological proximity of the network nodes, can there be any sort of influence on the evolution of the model during training</t>
+  </si>
+  <si>
+    <t>Convergence speed</t>
+  </si>
+  <si>
+    <t>The speed at which the model converges should be minimised, while the accuracy is maintained</t>
   </si>
   <si>
     <t>Privacy</t>
@@ -891,25 +1067,21 @@
 • Membership inference attacks (attacker uses the trained model to dedude the participation of specific members in the FL prcoess)</t>
   </si>
   <si>
-    <t>Scalability</t>
-  </si>
-  <si>
-    <t>A lot of the research has been done on limited scale implementations:
-• Some examples include the Google Gboard, with many millions of installs</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Non-Independent and Identically Distributed Data (Non-IID) data is a significant challenge if FL:
-</t>
-    </r>
-    <r>
-      <rPr>
+    <r>
+      <t xml:space="preserve">A lot of the research has been done on limited scale implementations:
+• Some examples include the Google Gboard, with many millions of installs
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Aptos Narrow"/>
         <family val="2"/>
-      </rPr>
-      <t>•</t>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Performance needs to remain consistent when working at scale</t>
     </r>
     <r>
       <rPr>
@@ -917,110 +1089,62 @@
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Models being updated with Independent and Identically Distributed (IID) data is a typical assumtion of FL
-</t>
-    </r>
-    <r>
-      <rPr>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>• But this is not what happens in real life
-• Assuming IID, and getting Non-IID can greatly increase the training complexity</t>
-    </r>
-  </si>
-  <si>
-    <t>Non-IID</t>
-  </si>
-  <si>
-    <t>Imblanced Data</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is the situation where the data distribution is different across different devices (clients or server)
-</t>
-    </r>
-    <r>
-      <rPr>
+      <t>The system as a whole should remain reliable</t>
+    </r>
+  </si>
+  <si>
+    <t>Main Area</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Clients participating in model learning can be offline, or on a slow, expensive connection
+• People have sought to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>•</t>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">reduce communication rounds
+</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> In the form of non-identical and independently distrinuted (non-IID) data, belonging to the devices
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">• Domain shift: where local datasets possess various characteristcs and features - these disparities can impact performance and convergence
-• An example would be two system to monitor accents, running the same model, with one device located in Cork, and another in Paris
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Imbalanced data distribution can lead to statistical heterogeneity</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Some clients can produce more data than others, and sometimes this difference can be significant, and this can be a challenge:
-• </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Imbalanced data distribution can lead to statistical heterogeneity</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-• Will lead to an increase in training complexity</t>
-    </r>
+      <t xml:space="preserve">• The ability of a client to process data fast is important
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Subarea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1126,8 +1250,39 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1149,8 +1304,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEF7C24"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1194,6 +1355,361 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1204,7 +1720,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1269,14 +1785,132 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1287,6 +1921,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEF7C24"/>
+      <color rgb="FFEBE115"/>
+      <color rgb="FFFFCC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1621,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="105" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1836,7 +2477,7 @@
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="17" t="s">
         <v>38</v>
       </c>
@@ -1856,7 +2497,7 @@
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="9" t="s">
         <v>41</v>
       </c>
@@ -1901,34 +2542,43 @@
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="9" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="10">
+        <v>50</v>
+      </c>
+      <c r="E13" s="60">
         <v>2023</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="20"/>
+    <row r="14" spans="1:8" s="3" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>13</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="61">
+        <v>2024</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="21"/>
       <c r="G15" s="20"/>
     </row>
@@ -2210,176 +2860,516 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8B0AD9-241F-48FB-91B9-FA2C6942572D}">
-  <dimension ref="C2:F13"/>
+  <dimension ref="B1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="120.21875" customWidth="1"/>
+    <col min="1" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="140.88671875" style="53" customWidth="1"/>
     <col min="6" max="6" width="8" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="2" t="s">
+    <row r="1" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C3" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="29" t="s">
+    <row r="2" spans="3:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>57</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="58"/>
+      <c r="D3" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>60</v>
       </c>
       <c r="F3" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C4" s="28"/>
-      <c r="D4" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="2">
-        <v>12</v>
+    <row r="4" spans="3:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="58"/>
+      <c r="D4" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C5" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>56</v>
+      <c r="C5" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>65</v>
       </c>
       <c r="F5" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C6" s="28"/>
-      <c r="D6" s="28" t="s">
+    <row r="6" spans="3:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="58"/>
+      <c r="D6" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C7" s="28"/>
-      <c r="D7" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>76</v>
+    <row r="7" spans="3:6" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="58"/>
+      <c r="D7" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>92</v>
       </c>
       <c r="F7" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C8" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>62</v>
+    <row r="8" spans="3:6" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="59"/>
+      <c r="D8" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="F8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="40"/>
+      <c r="D11" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="C9" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="29" t="s">
+    <row r="12" spans="3:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="40"/>
+      <c r="D12" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F12" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="43"/>
+      <c r="D13" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C10" s="28"/>
-      <c r="D10" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C11" s="28"/>
-      <c r="D11" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C12" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="2">
+    <row r="15" spans="3:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="40"/>
+      <c r="D15" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="43"/>
+      <c r="D16" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="3:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="C13" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="2">
-        <v>12</v>
-      </c>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="64"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="62"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="66"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="62"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="62"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="62"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="69"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="62"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="69"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="62"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="69"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="62"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="69"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="62"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="62"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="69"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="62"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="69"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="64"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="64"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="64"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="64"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="64"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="64"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="64"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="62"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="64"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="62"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="64"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="62"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="64"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="62"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="64"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="62"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="64"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="64"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="64"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="64"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="62"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="64"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="62"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="64"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="62"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="64"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="62"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="64"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="62"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="64"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="62"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="63"/>
+      <c r="E56" s="64"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="64"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="62"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="64"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="62"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="64"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="62"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="63"/>
+      <c r="E60" s="64"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="62"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="64"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="62"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="64"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="62"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="64"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="64"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="62"/>
+      <c r="C65" s="62"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="64"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="62"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="64"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="62"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="64"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="62"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="64"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C5:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B23D87B-BBF6-4F81-BEE9-EBBEA4BE4A13}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No changes to this, I just opened it and looked at some cells
</commit_message>
<xml_diff>
--- a/Article Searches/Reading.xlsx
+++ b/Article Searches/Reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulster-my.sharepoint.com/personal/o_fithcheallaigh-s_ulster_ac_uk/Documents/PhD/phd/Article Searches/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="629" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB06C783-84A7-4893-A3D2-9E71523E2C3D}"/>
+  <xr:revisionPtr revIDLastSave="630" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FFFD770-B9DB-48C1-B116-0AA2A3E72195}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,9 +719,6 @@
     </r>
   </si>
   <si>
-    <t>A systematic Review of Federted Leaning: Challenges, Aggregation Methodss, and Development Tools</t>
-  </si>
-  <si>
     <t>Badra Souhial Guendouzi</t>
   </si>
   <si>
@@ -1138,6 +1135,9 @@
   </si>
   <si>
     <t>Subarea</t>
+  </si>
+  <si>
+    <t>A systematic Review of Federted Leaning: Challenges, Aggregation Methods, and Development Tools</t>
   </si>
 </sst>
 </file>
@@ -1720,7 +1720,7 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1821,96 +1821,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2263,7 +2256,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="105" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2542,16 +2535,16 @@
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="54">
+        <v>2023</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="E13" s="60">
-        <v>2023</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="G13" s="16"/>
     </row>
@@ -2560,16 +2553,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="E14" s="55">
+        <v>2024</v>
+      </c>
+      <c r="F14" s="30" t="s">
         <v>53</v>
-      </c>
-      <c r="E14" s="61">
-        <v>2024</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>54</v>
       </c>
       <c r="G14" s="16"/>
     </row>
@@ -2860,7 +2853,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8B0AD9-241F-48FB-91B9-FA2C6942572D}">
-  <dimension ref="B1:F68"/>
+  <dimension ref="C1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -2871,485 +2864,271 @@
     <col min="1" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="140.88671875" style="53" customWidth="1"/>
+    <col min="5" max="5" width="140.88671875" style="50" customWidth="1"/>
     <col min="6" max="6" width="8" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="54" t="s">
-        <v>55</v>
+      <c r="C1" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>54</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="3:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="E2" s="44" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>58</v>
       </c>
       <c r="F2" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="3:6" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="58"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="43" t="s">
         <v>59</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>60</v>
       </c>
       <c r="F3" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="3:6" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="58"/>
+      <c r="C4" s="63"/>
       <c r="D4" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="28" t="s">
+    </row>
+    <row r="5" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="3:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="C5" s="57" t="s">
+      <c r="D5" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="E5" s="44" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>65</v>
       </c>
       <c r="F5" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="3:6" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="58"/>
+      <c r="C6" s="63"/>
       <c r="D6" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="31" t="s">
+    </row>
+    <row r="7" spans="3:6" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="63"/>
+      <c r="D7" s="38" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="58"/>
-      <c r="D7" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>92</v>
+      <c r="E7" s="46" t="s">
+        <v>91</v>
       </c>
       <c r="F7" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="3:6" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="59"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="42" t="s">
         <v>69</v>
-      </c>
-      <c r="E8" s="45" t="s">
-        <v>70</v>
       </c>
       <c r="F8" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="3:6" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="E9" s="47" t="s">
         <v>72</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>73</v>
       </c>
       <c r="F9" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="E10" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="51" t="s">
+    </row>
+    <row r="11" spans="3:6" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="65"/>
+      <c r="D11" s="32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="40"/>
-      <c r="D11" s="32" t="s">
+      <c r="E11" s="46" t="s">
         <v>77</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>78</v>
       </c>
       <c r="F11" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="3:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="40"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="46" t="s">
         <v>79</v>
-      </c>
-      <c r="E12" s="49" t="s">
-        <v>80</v>
       </c>
       <c r="F12" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="3:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="43"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="49" t="s">
         <v>81</v>
-      </c>
-      <c r="E13" s="52" t="s">
-        <v>82</v>
       </c>
       <c r="F13" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="3:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="E14" s="48" t="s">
         <v>84</v>
-      </c>
-      <c r="E14" s="51" t="s">
-        <v>85</v>
       </c>
       <c r="F14" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="3:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="40"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="46" t="s">
         <v>86</v>
-      </c>
-      <c r="E15" s="49" t="s">
-        <v>87</v>
       </c>
       <c r="F15" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="3:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="43"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="49" t="s">
         <v>88</v>
-      </c>
-      <c r="E16" s="52" t="s">
-        <v>89</v>
       </c>
       <c r="F16" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="44" t="s">
+    <row r="17" spans="3:6" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="42" t="s">
         <v>90</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>91</v>
       </c>
       <c r="F17" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="64"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="62"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="66"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="62"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="69"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="62"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="69"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="62"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="69"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="62"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="69"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="62"/>
-      <c r="C31" s="70"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="69"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="62"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="69"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="62"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="69"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="62"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="69"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="62"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="69"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="64"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="64"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="64"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="62"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="64"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="62"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="64"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="62"/>
-      <c r="C41" s="62"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="64"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="62"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="64"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="62"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="64"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="62"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="64"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="64"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="62"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="64"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B47" s="62"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="64"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B48" s="62"/>
-      <c r="C48" s="62"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="64"/>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="62"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="64"/>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="62"/>
-      <c r="C50" s="62"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="64"/>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B51" s="62"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="64"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="62"/>
-      <c r="C52" s="62"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="64"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="62"/>
-      <c r="C53" s="62"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="64"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="62"/>
-      <c r="C54" s="62"/>
-      <c r="D54" s="63"/>
-      <c r="E54" s="64"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="62"/>
-      <c r="C55" s="62"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="64"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="62"/>
-      <c r="C56" s="62"/>
-      <c r="D56" s="63"/>
-      <c r="E56" s="64"/>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="62"/>
-      <c r="C57" s="62"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="64"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="62"/>
-      <c r="C58" s="62"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="64"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="62"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="64"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="62"/>
-      <c r="C60" s="62"/>
-      <c r="D60" s="63"/>
-      <c r="E60" s="64"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="62"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="64"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="62"/>
-      <c r="C62" s="62"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="64"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="62"/>
-      <c r="C63" s="62"/>
-      <c r="D63" s="63"/>
-      <c r="E63" s="64"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" s="62"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="63"/>
-      <c r="E64" s="64"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B65" s="62"/>
-      <c r="C65" s="62"/>
-      <c r="D65" s="63"/>
-      <c r="E65" s="64"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" s="62"/>
-      <c r="C66" s="62"/>
-      <c r="D66" s="63"/>
-      <c r="E66" s="64"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="62"/>
-      <c r="C67" s="62"/>
-      <c r="D67" s="63"/>
-      <c r="E67" s="64"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="62"/>
-      <c r="C68" s="62"/>
-      <c r="D68" s="63"/>
-      <c r="E68" s="64"/>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="57"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="58"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="61"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="60"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="61"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="60"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="61"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="60"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="61"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="61"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="61"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="61"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="60"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>